<commit_message>
both parts sticked together, but still needs many improvements, as well as better integration between the parts
</commit_message>
<xml_diff>
--- a/Models/DEModel_modified.xlsx
+++ b/Models/DEModel_modified.xlsx
@@ -4854,11 +4854,7 @@
       <c r="N60" s="5" t="n"/>
       <c r="O60" s="4" t="n"/>
       <c r="Q60" s="5" t="n"/>
-      <c r="R60" s="5" t="inlineStr">
-        <is>
-          <t>[2020 660;2050 555]</t>
-        </is>
-      </c>
+      <c r="R60" s="5" t="n"/>
       <c r="S60" s="4" t="n"/>
       <c r="T60" s="5" t="n"/>
       <c r="U60" s="5" t="n"/>
@@ -4960,7 +4956,11 @@
       <c r="N62" s="5" t="n"/>
       <c r="O62" s="4" t="n"/>
       <c r="Q62" s="5" t="n"/>
-      <c r="R62" s="5" t="n"/>
+      <c r="R62" s="5" t="inlineStr">
+        <is>
+          <t>46.87216658103186</t>
+        </is>
+      </c>
       <c r="S62" s="4" t="n"/>
       <c r="T62" s="5" t="n"/>
       <c r="U62" s="5" t="n"/>

</xml_diff>

<commit_message>
moving the project from the notebook to .py files and creating the last parts necessary for the original graph, ready to create the UI and to modify it for the new use cases
</commit_message>
<xml_diff>
--- a/Models/DEModel_modified.xlsx
+++ b/Models/DEModel_modified.xlsx
@@ -4909,7 +4909,7 @@
         <v>104</v>
       </c>
       <c r="R61" s="5" t="n">
-        <v>3500</v>
+        <v>178.08</v>
       </c>
       <c r="S61" s="4" t="n"/>
       <c r="T61" s="5" t="n"/>
@@ -4956,11 +4956,7 @@
       <c r="N62" s="5" t="n"/>
       <c r="O62" s="4" t="n"/>
       <c r="Q62" s="5" t="n"/>
-      <c r="R62" s="5" t="inlineStr">
-        <is>
-          <t>46.87216658103186</t>
-        </is>
-      </c>
+      <c r="R62" s="5" t="n"/>
       <c r="S62" s="4" t="n"/>
       <c r="T62" s="5" t="n"/>
       <c r="U62" s="5" t="n"/>

</xml_diff>